<commit_message>
minor : pisah import barang modal
</commit_message>
<xml_diff>
--- a/public/excel/barangmasuk.xlsx
+++ b/public/excel/barangmasuk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikms\prod-inventory\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikms\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{165E45AF-F499-4C84-B631-307BA43EEC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A170D17C-53F5-4F92-B8D5-AD4AA6DBFE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="4875" windowWidth="20460" windowHeight="11490" xr2:uid="{C7E7DE1C-4457-4699-B246-BE3E90BC3F5A}"/>
+    <workbookView xWindow="-20610" yWindow="2025" windowWidth="20730" windowHeight="11760" xr2:uid="{C7E7DE1C-4457-4699-B246-BE3E90BC3F5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>nama_barang</t>
   </si>
@@ -48,13 +48,19 @@
     <t>harga</t>
   </si>
   <si>
-    <t>Akrilik (130x60x0,3)</t>
-  </si>
-  <si>
-    <t>Mitra Komputer</t>
-  </si>
-  <si>
-    <t>Lampu Cabe</t>
+    <t>satuan</t>
+  </si>
+  <si>
+    <t>pak</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Contoh Suplayer</t>
+  </si>
+  <si>
+    <t>Contoh Barang</t>
   </si>
 </sst>
 </file>
@@ -430,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5088AA-180D-408D-8019-835AABDB0DB8}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,36 +462,63 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>500</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3">
-        <v>5000</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
         <v>500</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Core : add print qrcode
</commit_message>
<xml_diff>
--- a/public/excel/barangmasuk.xlsx
+++ b/public/excel/barangmasuk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikms\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikms\prod-inventory\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A170D17C-53F5-4F92-B8D5-AD4AA6DBFE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7DE966-4B2D-4E1D-AA61-A1E5F9DDC09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2025" windowWidth="20730" windowHeight="11760" xr2:uid="{C7E7DE1C-4457-4699-B246-BE3E90BC3F5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E7DE1C-4457-4699-B246-BE3E90BC3F5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>nama_barang</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Contoh Barang</t>
+  </si>
+  <si>
+    <t>sumber_dana</t>
+  </si>
+  <si>
+    <t>Dana BOS</t>
   </si>
 </sst>
 </file>
@@ -112,13 +118,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -436,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5088AA-180D-408D-8019-835AABDB0DB8}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,9 +456,10 @@
     <col min="1" max="1" width="33.140625" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +475,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -482,8 +495,11 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -499,8 +515,11 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -515,6 +534,9 @@
       </c>
       <c r="E4" t="s">
         <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>